<commit_message>
Added subscribes and assinged functions.
</commit_message>
<xml_diff>
--- a/src/Excel_files/all_username.xlsx
+++ b/src/Excel_files/all_username.xlsx
@@ -15,18 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>12424324432dddfdf</t>
+    <t>bdvb(12)</t>
   </si>
   <si>
-    <t>23121dfsdff</t>
+    <t>gggggg(gg)</t>
   </si>
   <si>
-    <t>243ffgfgfgf</t>
+    <t>llll(ll)</t>
+  </si>
+  <si>
+    <t>Xiao(xiao)</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -390,6 +393,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added upload and owner function.
</commit_message>
<xml_diff>
--- a/src/Excel_files/all_username.xlsx
+++ b/src/Excel_files/all_username.xlsx
@@ -15,18 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>username</t>
-  </si>
-  <si>
-    <t>bdvb(12)</t>
-  </si>
-  <si>
-    <t>gggggg(gg)</t>
-  </si>
-  <si>
-    <t>llll(ll)</t>
   </si>
   <si>
     <t>Xiao(xiao)</t>
@@ -365,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -383,21 +374,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>